<commit_message>
Added controller for search, spell check, frequency count
</commit_message>
<xml_diff>
--- a/FrequencyCount.xlsx
+++ b/FrequencyCount.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Search Word</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>party</t>
+  </si>
+  <si>
+    <t>back</t>
   </si>
 </sst>
 </file>
@@ -74,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -101,7 +104,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="4">
@@ -120,6 +123,14 @@
         <v>15.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>2.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>